<commit_message>
Jobsheet 8 - Tugas 1 - Implementasi File Upload untuk Import Data
</commit_message>
<xml_diff>
--- a/Week_8/POS/public/template_barang.xlsx
+++ b/Week_8/POS/public/template_barang.xlsx
@@ -401,7 +401,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,7 +432,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>

</xml_diff>